<commit_message>
Training Data Set Complete, Edited Function
</commit_message>
<xml_diff>
--- a/2012.xlsx
+++ b/2012.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NMath\Desktop\keras\Data-Analysis-Project-2022-T20-World-Cup-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96FE94D8-6D18-4B3D-8EC0-FA8ECB2EEA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFCC5FA-8434-47F1-915B-951FEEBBF628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB098E79-2232-45FB-BD9A-FECD7A2C2C1E}"/>
+    <workbookView xWindow="-5316" yWindow="3648" windowWidth="15576" windowHeight="8076" xr2:uid="{EB098E79-2232-45FB-BD9A-FECD7A2C2C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Names</t>
   </si>
@@ -63,6 +63,51 @@
   </si>
   <si>
     <t>IntExp</t>
+  </si>
+  <si>
+    <t>Darren Sammy</t>
+  </si>
+  <si>
+    <t>Dwayne Bravo</t>
+  </si>
+  <si>
+    <t>Samuel Badree</t>
+  </si>
+  <si>
+    <t>Darren Bravo</t>
+  </si>
+  <si>
+    <t>Johnson Charles</t>
+  </si>
+  <si>
+    <t>Fidel Edwards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chris Gayle </t>
+  </si>
+  <si>
+    <t>Sunil Narine</t>
+  </si>
+  <si>
+    <t>Kieron Pollard</t>
+  </si>
+  <si>
+    <t>Denesh Ramdin</t>
+  </si>
+  <si>
+    <t>Ravi Rampaul</t>
+  </si>
+  <si>
+    <t>Andre Russell</t>
+  </si>
+  <si>
+    <t>Marlon Samuels</t>
+  </si>
+  <si>
+    <t>Lendl Simmons</t>
+  </si>
+  <si>
+    <t>Dwayne Smith</t>
   </si>
 </sst>
 </file>
@@ -414,13 +459,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C5A3E5-6A3C-473E-B84E-9DA0C705144A}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -449,6 +497,441 @@
       </c>
       <c r="I1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>29</v>
+      </c>
+      <c r="I2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>27</v>
+      </c>
+      <c r="I3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>17</v>
+      </c>
+      <c r="I7">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>23</v>
+      </c>
+      <c r="I8">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>24</v>
+      </c>
+      <c r="I10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>26</v>
+      </c>
+      <c r="I11">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>15</v>
+      </c>
+      <c r="I14">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>